<commit_message>
add docstring to each class
</commit_message>
<xml_diff>
--- a/tests/excel.xlsx
+++ b/tests/excel.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="page_0" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="page_1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data 2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>